<commit_message>
updating SS concentrations from LISST data
</commit_message>
<xml_diff>
--- a/GSD/Water Samples/LaJara_LISST_GSD_Summer2021.xlsx
+++ b/GSD/Water Samples/LaJara_LISST_GSD_Summer2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vandalsuidaho-my.sharepoint.com/personal/huck4481_vandals_uidaho_edu/Documents/Desktop/Research/Data/La Jara/LISST GSD/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\GSD\Water Samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{2AD361F5-9DB5-4552-A58B-67D9F26E690C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90938A94-1760-4CA1-82CB-4FCEFE5203BC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C11BC9-1552-4EE5-9018-43E4E3526658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-180" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{1DA23FE7-BAAC-465E-A779-A09567432D19}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1DA23FE7-BAAC-465E-A779-A09567432D19}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiment" sheetId="1" r:id="rId1"/>
@@ -318,7 +318,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -381,6 +381,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1128,7 +1131,7 @@
   <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1170,7 +1173,9 @@
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
+      <c r="B2" s="22">
+        <v>0.65972222222222221</v>
+      </c>
       <c r="C2" s="5">
         <v>117</v>
       </c>
@@ -1192,7 +1197,9 @@
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="3"/>
+      <c r="B3" s="22">
+        <v>0.67291666666666661</v>
+      </c>
       <c r="C3" s="5">
         <v>200</v>
       </c>
@@ -1214,7 +1221,9 @@
       <c r="A4" s="2">
         <v>5</v>
       </c>
-      <c r="B4" s="3"/>
+      <c r="B4" s="22">
+        <v>0.69444444444444453</v>
+      </c>
       <c r="C4" s="5">
         <v>150</v>
       </c>
@@ -1236,7 +1245,9 @@
       <c r="A5" s="2">
         <v>6</v>
       </c>
-      <c r="B5" s="3"/>
+      <c r="B5" s="22">
+        <v>0.70486111111111116</v>
+      </c>
       <c r="C5" s="5">
         <v>125</v>
       </c>
@@ -1258,7 +1269,9 @@
       <c r="A6" s="2">
         <v>10</v>
       </c>
-      <c r="B6" s="3"/>
+      <c r="B6" s="22">
+        <v>0.80486111111111114</v>
+      </c>
       <c r="C6" s="5">
         <v>117</v>
       </c>
@@ -1279,7 +1292,9 @@
       <c r="A7" s="2">
         <v>18</v>
       </c>
-      <c r="B7" s="3"/>
+      <c r="B7" s="22">
+        <v>0.87638888888888899</v>
+      </c>
       <c r="C7" s="5">
         <v>117</v>
       </c>
@@ -1323,7 +1338,9 @@
       <c r="A10" s="2">
         <v>1</v>
       </c>
-      <c r="B10" s="3"/>
+      <c r="B10" s="22">
+        <v>0.62083333333333335</v>
+      </c>
       <c r="C10" s="5">
         <v>117</v>
       </c>
@@ -1344,7 +1361,9 @@
       <c r="A11" s="2">
         <v>3</v>
       </c>
-      <c r="B11" s="3"/>
+      <c r="B11" s="22">
+        <v>0.62638888888888888</v>
+      </c>
       <c r="C11" s="5">
         <v>117</v>
       </c>
@@ -1365,7 +1384,9 @@
       <c r="A12" s="2">
         <v>8</v>
       </c>
-      <c r="B12" s="3"/>
+      <c r="B12" s="22">
+        <v>0.67569444444444438</v>
+      </c>
       <c r="C12" s="5">
         <v>150</v>
       </c>
@@ -1387,7 +1408,9 @@
       <c r="A13" s="2">
         <v>11</v>
       </c>
-      <c r="B13" s="3"/>
+      <c r="B13" s="22">
+        <v>0.70694444444444438</v>
+      </c>
       <c r="C13" s="5">
         <v>117</v>
       </c>
@@ -1408,7 +1431,9 @@
       <c r="A14" s="2">
         <v>15</v>
       </c>
-      <c r="B14" s="3"/>
+      <c r="B14" s="22">
+        <v>0.74861111111111101</v>
+      </c>
       <c r="C14" s="5">
         <v>117</v>
       </c>
@@ -1429,7 +1454,9 @@
       <c r="A15" s="2">
         <v>24</v>
       </c>
-      <c r="B15" s="3"/>
+      <c r="B15" s="22">
+        <v>0.84236111111111101</v>
+      </c>
       <c r="C15" s="5">
         <v>117</v>
       </c>
@@ -1893,13 +1920,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="G26:I26"/>
     <mergeCell ref="A17:G17"/>
     <mergeCell ref="A20:C20"/>
     <mergeCell ref="A24:C24"/>
@@ -1908,6 +1928,13 @@
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="D20:F20"/>
     <mergeCell ref="D24:F24"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="G26:I26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>